<commit_message>
Added more results, added class sampling to chipper
</commit_message>
<xml_diff>
--- a/results/results_dota.xlsx
+++ b/results/results_dota.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\school\e2cnn_experiments\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758BC506-C399-4399-A9D9-461B9C9CA971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E0418C-9E11-4A5B-BE36-886E8FA45628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{484F53C8-DA1C-4908-B869-EDBB5FA70F7E}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="22950" windowHeight="13770" xr2:uid="{484F53C8-DA1C-4908-B869-EDBB5FA70F7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1092,7 +1092,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
-          <c:min val="40"/>
+          <c:min val="50"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3965,14 +3965,14 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>